<commit_message>
belajar PSBO praktikum 9
</commit_message>
<xml_diff>
--- a/CodeMetKuan/kuliah/metkuan 2 110914/2c Contoh RAL faktorial.xlsx
+++ b/CodeMetKuan/kuliah/metkuan 2 110914/2c Contoh RAL faktorial.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Belajar\TugasKuliah\CodeMetKuan\kuliah\metkuan 2 110914\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="75" windowWidth="15120" windowHeight="7995"/>
   </bookViews>
@@ -11,7 +16,7 @@
     <sheet name="data ke R" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -365,6 +370,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -412,7 +420,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -447,7 +455,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -658,8 +666,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:L5"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="S15" sqref="S15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1338,11 +1346,11 @@
         <v>3.8055555555556566</v>
       </c>
       <c r="R16" s="21">
-        <f t="shared" ref="R16:R18" si="12">Q16/Q$19</f>
+        <f>Q16/Q$19</f>
         <v>7.2105263157897515</v>
       </c>
       <c r="S16" s="20">
-        <f t="shared" ref="S16:S18" si="13">_xlfn.F.DIST.RT(R16,O16,O$19)</f>
+        <f t="shared" ref="S16:S18" si="12">_xlfn.F.DIST.RT(R16,O16,O$19)</f>
         <v>1.2942626554820935E-3</v>
       </c>
     </row>
@@ -1400,11 +1408,11 @@
         <v>123.69444444444457</v>
       </c>
       <c r="R17" s="21">
+        <f t="shared" ref="R16:R18" si="13">Q17/Q$19</f>
+        <v>234.36842105263463</v>
+      </c>
+      <c r="S17" s="20">
         <f t="shared" si="12"/>
-        <v>234.36842105263463</v>
-      </c>
-      <c r="S17" s="20">
-        <f t="shared" si="13"/>
         <v>1.7830128392081718E-16</v>
       </c>
     </row>
@@ -1463,11 +1471,11 @@
         <v>0.47222222222217169</v>
       </c>
       <c r="R18" s="21">
+        <f t="shared" si="13"/>
+        <v>0.89473684210517812</v>
+      </c>
+      <c r="S18" s="20">
         <f t="shared" si="12"/>
-        <v>0.89473684210517812</v>
-      </c>
-      <c r="S18" s="20">
-        <f t="shared" si="13"/>
         <v>0.51449994089903373</v>
       </c>
     </row>
@@ -1519,7 +1527,7 @@
         <v>12.666666666666515</v>
       </c>
       <c r="Q19" s="21">
-        <f t="shared" si="11"/>
+        <f>P19/O19</f>
         <v>0.52777777777777146</v>
       </c>
       <c r="R19" s="21"/>

</xml_diff>